<commit_message>
Charge 15 C05 - updated inventory and weight out charge
</commit_message>
<xml_diff>
--- a/Charge 14 - C04.xlsx
+++ b/Charge 14 - C04.xlsx
@@ -831,19 +831,19 @@
     <t xml:space="preserve">Will have long, thin pieces that are easy to clean and fit in a crucible. </t>
   </si>
   <si>
-    <t>Held at 510 for 30 seconds</t>
-  </si>
-  <si>
     <t>Then stirred melt before casting</t>
   </si>
   <si>
     <t>Stirred melt at high temp of each heating cycle</t>
   </si>
   <si>
-    <t>Held melt at 510C for 30 seconds and stirred just before casting</t>
-  </si>
-  <si>
     <t>Charge 14 - C04</t>
+  </si>
+  <si>
+    <t>Held at 450 for 30 seconds</t>
+  </si>
+  <si>
+    <t>Held melt at 450C for 30 seconds and stirred just before casting</t>
   </si>
 </sst>
 </file>
@@ -4911,7 +4911,7 @@
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="173" t="str">
         <f>"Actual  " &amp; 'Charge 14'!I3</f>
-        <v>Actual  Mg0Ca100</v>
+        <v>Actual  Mg65Zn30Ca5</v>
       </c>
       <c r="B3" s="174"/>
       <c r="C3" s="174"/>
@@ -4973,17 +4973,17 @@
       <c r="A6" s="26">
         <v>1</v>
       </c>
-      <c r="B6" s="105" t="str">
+      <c r="B6" s="105">
         <f>IF('Charge 14'!B14=0, "-", 'Charge 14'!B14)</f>
-        <v>-</v>
-      </c>
-      <c r="C6" s="137" t="str">
+        <v>6.2190000000000003</v>
+      </c>
+      <c r="C6" s="137">
         <f>IF('Charge 14'!E14=0,"-",'Charge 14'!E14)</f>
-        <v>-</v>
+        <v>9.782</v>
       </c>
       <c r="D6" s="137">
         <f>IF('Charge 14'!H14=0, "-", 'Charge 14'!H14)</f>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="E6" s="137" t="str">
         <f>IF('Charge 14'!K14=0, "-", 'Charge 14'!K14)</f>
@@ -4995,7 +4995,7 @@
       </c>
       <c r="G6" s="138">
         <f>COUNTIF(B6:B20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="131" t="str">
         <f>B4</f>
@@ -5006,13 +5006,13 @@
       <c r="A7" s="27">
         <v>2</v>
       </c>
-      <c r="B7" s="108" t="str">
+      <c r="B7" s="108">
         <f>IF('Charge 14'!B15=0, "-", 'Charge 14'!B15)</f>
-        <v>-</v>
-      </c>
-      <c r="C7" s="107" t="str">
+        <v>7.3159999999999998</v>
+      </c>
+      <c r="C7" s="107">
         <f>IF('Charge 14'!E15=0,"-",'Charge 14'!E15)</f>
-        <v>-</v>
+        <v>20.515000000000001</v>
       </c>
       <c r="D7" s="107" t="str">
         <f>IF('Charge 14'!H15=0, "-", 'Charge 14'!H15)</f>
@@ -5028,7 +5028,7 @@
       </c>
       <c r="G7" s="106">
         <f>COUNTIF(C6:C20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="151" t="str">
         <f>C4</f>
@@ -5039,9 +5039,9 @@
       <c r="A8" s="27">
         <v>3</v>
       </c>
-      <c r="B8" s="108" t="str">
+      <c r="B8" s="108">
         <f>IF('Charge 14'!B16=0, "-", 'Charge 14'!B16)</f>
-        <v>-</v>
+        <v>10.866</v>
       </c>
       <c r="C8" s="107" t="str">
         <f>IF('Charge 14'!E16=0,"-",'Charge 14'!E16)</f>
@@ -5160,7 +5160,7 @@
       </c>
       <c r="G11" s="160">
         <f>COUNTIF(B6:F20, "&lt;&gt;-")</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H11" s="153" t="str">
         <f>G4</f>
@@ -5407,15 +5407,15 @@
       </c>
       <c r="B21" s="77">
         <f>SUM(B6:B20)</f>
-        <v>0</v>
+        <v>24.401</v>
       </c>
       <c r="C21" s="37">
         <f>SUM(C6:C20)</f>
-        <v>0</v>
+        <v>30.297000000000001</v>
       </c>
       <c r="D21" s="69">
         <f>SUM(D6:D20)</f>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="E21" s="69">
         <f>SUM(E6:E20)</f>
@@ -5427,7 +5427,7 @@
       </c>
       <c r="G21" s="144">
         <f>SUM(B21:F21)</f>
-        <v>3.052</v>
+        <v>57.792999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5436,15 +5436,15 @@
       </c>
       <c r="B22" s="145">
         <f>'Charge 14'!F4</f>
-        <v>24.061</v>
+        <v>24.404</v>
       </c>
       <c r="C22" s="135">
         <f>'Charge 14'!F5</f>
-        <v>29.873000000000001</v>
+        <v>30.298999999999999</v>
       </c>
       <c r="D22" s="135">
         <f>'Charge 14'!F6</f>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="E22" s="135">
         <f>'Charge 14'!F7</f>
@@ -5456,7 +5456,7 @@
       </c>
       <c r="G22" s="70">
         <f>SUM(B22:F22)</f>
-        <v>56.985999999999997</v>
+        <v>57.798000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5465,11 +5465,11 @@
       </c>
       <c r="B23" s="146">
         <f>B21-B22</f>
-        <v>-24.061</v>
+        <v>-3.0000000000001137E-3</v>
       </c>
       <c r="C23" s="140">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
-        <v>-29.873000000000001</v>
+        <v>-1.9999999999988916E-3</v>
       </c>
       <c r="D23" s="140">
         <f t="shared" si="0"/>
@@ -5485,7 +5485,7 @@
       </c>
       <c r="G23" s="113">
         <f t="shared" si="0"/>
-        <v>-53.933999999999997</v>
+        <v>-5.000000000002558E-3</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -5511,7 +5511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G1"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5534,7 +5534,7 @@
   <sheetData>
     <row r="1" spans="1:28" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="176" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B1" s="176"/>
       <c r="C1" s="176"/>
@@ -5581,7 +5581,7 @@
       </c>
       <c r="I3" s="62" t="str">
         <f>Q4 &amp; ROUND(N4,3)*100 &amp; IF(N5=0, "", Q5 &amp; ROUND(N5,3)*100) &amp; IF(N6=0, "", Q6 &amp; ROUND(N6,3)*100) &amp; IF(N7=0, "", Q7 &amp; ROUND(N7,3)*100) &amp; IF(N8=0, "", Q8 &amp; ROUND(N8,3)*100)</f>
-        <v>Mg0Ca100</v>
+        <v>Mg65Zn30Ca5</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="s">
@@ -5674,11 +5674,11 @@
       </c>
       <c r="F4" s="69">
         <f>IF($F$9=0, ROUND($F$10*E4, 3), ROUND(E4*$F$9, 3))</f>
-        <v>24.061</v>
+        <v>24.404</v>
       </c>
       <c r="G4" s="70">
         <f>IFERROR(F4/U4, 0)</f>
-        <v>13.844073647871117</v>
+        <v>14.041426927502878</v>
       </c>
       <c r="I4" s="71" t="str">
         <f>$Q$4</f>
@@ -5687,19 +5687,19 @@
       <c r="J4" s="26"/>
       <c r="K4" s="72">
         <f>B29</f>
-        <v>0</v>
+        <v>24.401</v>
       </c>
       <c r="L4" s="73">
         <f>K4/$K$9</f>
-        <v>0</v>
+        <v>0.42221376291246343</v>
       </c>
       <c r="M4" s="23">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>0</v>
+        <v>1.7371477593600634E-2</v>
       </c>
       <c r="N4" s="115">
         <f>M4/$M$9</f>
-        <v>0</v>
+        <v>0.64999138395731593</v>
       </c>
       <c r="P4" s="15">
         <v>1</v>
@@ -5771,11 +5771,11 @@
       </c>
       <c r="F5" s="69">
         <f t="shared" ref="F5:F8" si="0">IF($F$9=0, ROUND($F$10*E5, 3), ROUND(E5*$F$9, 3))</f>
-        <v>29.873000000000001</v>
+        <v>30.298999999999999</v>
       </c>
       <c r="G5" s="70">
         <f>IFERROR(F5/U5, 0)</f>
-        <v>4.1838935574229694</v>
+        <v>4.2435574229691877</v>
       </c>
       <c r="I5" s="71" t="str">
         <f>$Q$5</f>
@@ -5784,19 +5784,19 @@
       <c r="J5" s="27"/>
       <c r="K5" s="75">
         <f>E29</f>
-        <v>0</v>
+        <v>30.297000000000001</v>
       </c>
       <c r="L5" s="76">
         <f>K5/$K$9</f>
-        <v>0</v>
+        <v>0.52423303860329107</v>
       </c>
       <c r="M5" s="24">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>0</v>
+        <v>8.0180024869733416E-3</v>
       </c>
       <c r="N5" s="116">
         <f>M5/$M$9</f>
-        <v>0</v>
+        <v>0.30001089458278912</v>
       </c>
       <c r="P5" s="15">
         <v>2</v>
@@ -5868,11 +5868,11 @@
       </c>
       <c r="F6" s="69">
         <f t="shared" si="0"/>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="G6" s="70">
         <f>IFERROR(F6/U6, 0)</f>
-        <v>1.9690322580645161</v>
+        <v>1.9967741935483871</v>
       </c>
       <c r="I6" s="71" t="str">
         <f>$Q$6</f>
@@ -5881,19 +5881,19 @@
       <c r="J6" s="27"/>
       <c r="K6" s="77">
         <f>H29</f>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="L6" s="76">
         <f>K6/$K$9</f>
-        <v>1</v>
+        <v>5.3553198484245501E-2</v>
       </c>
       <c r="M6" s="24">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>2.4951344877488894E-2</v>
+        <v>1.336224324673025E-3</v>
       </c>
       <c r="N6" s="116">
         <f>M6/$M$9</f>
-        <v>1</v>
+        <v>4.9997721459894874E-2</v>
       </c>
       <c r="P6" s="15">
         <v>3</v>
@@ -6161,7 +6161,7 @@
       </c>
       <c r="G9" s="144">
         <f>SUM(G4:G8)</f>
-        <v>19.996999463358602</v>
+        <v>20.281758544020452</v>
       </c>
       <c r="I9" s="82"/>
       <c r="J9" s="79" t="s">
@@ -6169,7 +6169,7 @@
       </c>
       <c r="K9" s="117">
         <f>SUM(K4:K8)</f>
-        <v>3.052</v>
+        <v>57.792999999999999</v>
       </c>
       <c r="L9" s="83">
         <f>SUM(L4:L8)</f>
@@ -6177,11 +6177,11 @@
       </c>
       <c r="M9" s="118">
         <f>SUM(M4:M8)</f>
-        <v>2.4951344877488894E-2</v>
+        <v>2.6725704405247002E-2</v>
       </c>
       <c r="N9" s="84">
         <f>SUM(N4:N8)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>111</v>
@@ -6223,10 +6223,10 @@
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F10" s="158">
         <f>G10*U9</f>
-        <v>56.985750000000003</v>
+        <v>57.798000000000002</v>
       </c>
       <c r="G10" s="9">
-        <v>19.995000000000001</v>
+        <v>20.28</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="26.25" x14ac:dyDescent="0.4">
@@ -6332,7 +6332,7 @@
       </c>
       <c r="B14" s="106">
         <f>A!C2</f>
-        <v>0</v>
+        <v>6.2190000000000003</v>
       </c>
       <c r="C14" s="107"/>
       <c r="D14" s="126">
@@ -6340,7 +6340,7 @@
       </c>
       <c r="E14" s="106">
         <f>B!C2</f>
-        <v>0</v>
+        <v>9.782</v>
       </c>
       <c r="F14" s="107"/>
       <c r="G14" s="126">
@@ -6348,7 +6348,7 @@
       </c>
       <c r="H14" s="106">
         <f>'C'!C2</f>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="I14" s="107"/>
       <c r="J14" s="126">
@@ -6385,7 +6385,7 @@
       </c>
       <c r="B15" s="106">
         <f>A!C3</f>
-        <v>0</v>
+        <v>7.3159999999999998</v>
       </c>
       <c r="C15" s="107"/>
       <c r="D15" s="126">
@@ -6393,7 +6393,7 @@
       </c>
       <c r="E15" s="106">
         <f>B!C3</f>
-        <v>0</v>
+        <v>20.515000000000001</v>
       </c>
       <c r="F15" s="107"/>
       <c r="G15" s="126">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="B16" s="106">
         <f>A!C4</f>
-        <v>0</v>
+        <v>10.866</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="126">
@@ -6582,7 +6582,7 @@
         <v>97</v>
       </c>
       <c r="Q18" s="8">
-        <v>510</v>
+        <v>450</v>
       </c>
       <c r="R18" s="10" t="s">
         <v>98</v>
@@ -6638,7 +6638,7 @@
       </c>
       <c r="Q19" s="8"/>
       <c r="R19" s="10" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="S19" s="7"/>
       <c r="T19" s="8"/>
@@ -6691,7 +6691,7 @@
       </c>
       <c r="Q20" s="8"/>
       <c r="R20" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S20" s="7"/>
       <c r="T20" s="8"/>
@@ -7050,7 +7050,7 @@
       </c>
       <c r="B29" s="110">
         <f>SUM(B14:B28)</f>
-        <v>0</v>
+        <v>24.401</v>
       </c>
       <c r="C29" s="107"/>
       <c r="D29" s="109" t="s">
@@ -7058,7 +7058,7 @@
       </c>
       <c r="E29" s="111">
         <f>SUM(E14:E28)</f>
-        <v>0</v>
+        <v>30.297000000000001</v>
       </c>
       <c r="F29" s="107"/>
       <c r="G29" s="109" t="s">
@@ -7066,7 +7066,7 @@
       </c>
       <c r="H29" s="110">
         <f>SUM(H14:H28)</f>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="I29" s="107"/>
       <c r="J29" s="109" t="s">
@@ -7091,7 +7091,7 @@
       </c>
       <c r="B30" s="113">
         <f>B29-$F$4</f>
-        <v>-24.061</v>
+        <v>-3.0000000000001137E-3</v>
       </c>
       <c r="C30" s="114"/>
       <c r="D30" s="112" t="s">
@@ -7099,7 +7099,7 @@
       </c>
       <c r="E30" s="113">
         <f>E29-$F$5</f>
-        <v>-29.873000000000001</v>
+        <v>-1.9999999999988916E-3</v>
       </c>
       <c r="F30" s="114"/>
       <c r="G30" s="112" t="s">
@@ -7205,7 +7205,7 @@
       <c r="K34" s="43"/>
       <c r="L34" s="43"/>
       <c r="M34" s="43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N34" s="43"/>
       <c r="O34" s="43"/>
@@ -7239,7 +7239,7 @@
       <c r="K35" s="49"/>
       <c r="L35" s="43"/>
       <c r="M35" s="43" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N35" s="43"/>
       <c r="O35" s="43"/>
@@ -8507,7 +8507,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -8545,34 +8545,34 @@
         <v>6.2190000000000003</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
+        <v>6.2190000000000003</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>24.401</v>
       </c>
       <c r="E2" s="127" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="129">
         <f>'Charge 14'!F4</f>
-        <v>24.061</v>
+        <v>24.404</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="166">
-        <v>6.7640000000000002</v>
+        <v>7.3159999999999998</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.3159999999999998</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="127" t="s">
@@ -8580,19 +8580,19 @@
       </c>
       <c r="F3" s="129">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>24.401</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="166">
-        <v>7.3159999999999998</v>
+        <v>10.866</v>
       </c>
       <c r="B4" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>10.866</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="127" t="s">
@@ -8600,43 +8600,43 @@
       </c>
       <c r="F4" s="129">
         <f>F3-F2</f>
-        <v>-24.061</v>
+        <v>-3.0000000000001137E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="166">
-        <v>9.2379999999999995</v>
+        <v>6.7640000000000002</v>
       </c>
       <c r="B5" s="125">
         <v>0</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="166">
-        <v>10.641999999999999</v>
+        <v>9.2379999999999995</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="167"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="166">
-        <v>10.866</v>
+        <v>10.641999999999999</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8646,9 +8646,10 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="167"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="166"/>
@@ -8656,7 +8657,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8666,7 +8667,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8676,7 +8677,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8686,7 +8687,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8696,7 +8697,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8706,7 +8707,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8716,7 +8717,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8726,7 +8727,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8736,7 +8737,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8746,7 +8747,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8756,7 +8757,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8766,7 +8767,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8776,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8786,7 +8787,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8796,7 +8797,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8806,7 +8807,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8816,7 +8817,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8826,7 +8827,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8836,7 +8837,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8846,7 +8847,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8856,7 +8857,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8866,7 +8867,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8876,7 +8877,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8886,7 +8887,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8896,7 +8897,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8906,7 +8907,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8916,7 +8917,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8926,7 +8927,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8936,7 +8937,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8946,7 +8947,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8956,7 +8957,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8966,7 +8967,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8976,7 +8977,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8986,7 +8987,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8996,7 +8997,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9006,7 +9007,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9016,7 +9017,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9026,7 +9027,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9036,7 +9037,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9046,7 +9047,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9056,7 +9057,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9066,7 +9067,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9076,14 +9077,14 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9100,7 +9101,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9138,52 +9139,52 @@
         <v>9.782</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
+        <v>9.782</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>30.297000000000001</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="51">
         <f>'Charge 14'!F5</f>
-        <v>29.873000000000001</v>
+        <v>30.298999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="125">
-        <v>12.731</v>
+        <v>20.515000000000001</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>20.515000000000001</v>
       </c>
       <c r="E3" s="50" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>30.297000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="125">
-        <v>12.920999999999999</v>
+        <v>12.731</v>
       </c>
       <c r="B4" s="125">
         <v>0</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="50" t="s">
@@ -9191,90 +9192,90 @@
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-29.873000000000001</v>
+        <v>-1.9999999999988916E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="125">
-        <v>14.746</v>
+        <v>12.920999999999999</v>
       </c>
       <c r="B5" s="125">
         <v>0</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="125">
-        <v>16.824999999999999</v>
+        <v>14.746</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="125">
-        <v>17.745999999999999</v>
+        <v>16.824999999999999</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="125">
-        <v>19.539000000000001</v>
+        <v>17.745999999999999</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="125">
-        <v>19.594999999999999</v>
+        <v>19.539000000000001</v>
       </c>
       <c r="B9" s="125">
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="125">
-        <v>20.327999999999999</v>
+        <v>19.594999999999999</v>
       </c>
       <c r="B10" s="125">
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="125">
-        <v>20.693000000000001</v>
+        <v>20.327999999999999</v>
       </c>
       <c r="B11" s="125">
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9286,7 +9287,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9298,7 +9299,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9308,7 +9309,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9318,7 +9319,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9328,7 +9329,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9338,7 +9339,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9348,7 +9349,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9358,7 +9359,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9368,7 +9369,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9378,7 +9379,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9388,7 +9389,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9398,7 +9399,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9408,7 +9409,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9418,7 +9419,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9428,7 +9429,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9438,7 +9439,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9448,7 +9449,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9458,7 +9459,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9468,7 +9469,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9478,7 +9479,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9488,7 +9489,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9498,7 +9499,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9508,7 +9509,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9518,7 +9519,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9528,7 +9529,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9538,7 +9539,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9548,7 +9549,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9558,7 +9559,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9568,7 +9569,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9578,7 +9579,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9588,7 +9589,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9598,7 +9599,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9608,7 +9609,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9618,7 +9619,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9628,7 +9629,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9638,7 +9639,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9648,7 +9649,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9658,7 +9659,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9668,7 +9669,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9678,14 +9679,14 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9702,7 +9703,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9737,25 +9738,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="B2" s="125">
         <v>1</v>
       </c>
       <c r="C2">
         <f>IF(A2=0, 0, A2*B2)</f>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="51">
         <f>'Charge 14'!F6</f>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9772,7 +9773,7 @@
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>3.052</v>
+        <v>3.0950000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>